<commit_message>
Upload Source Code Bo Sung Khoa
</commit_message>
<xml_diff>
--- a/CAPSTONE-PhanCong-TranHuuPhuoc-TranDangKhoa.xlsx
+++ b/CAPSTONE-PhanCong-TranHuuPhuoc-TranDangKhoa.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phuoc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive\Desktop\capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5394AB-923D-4F60-8D4A-CDAABD524001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874FC98C-CAE7-437C-81AD-851EEDEDDDFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4AF2F624-0AE2-4AE2-852F-07B8860B0E06}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11835" xr2:uid="{4AF2F624-0AE2-4AE2-852F-07B8860B0E06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="32">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -121,13 +121,19 @@
   </si>
   <si>
     <t>Swiper JS</t>
+  </si>
+  <si>
+    <t>28/04/2025</t>
+  </si>
+  <si>
+    <t>Back To Top</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +158,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -253,9 +265,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -293,7 +305,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -399,7 +411,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -541,7 +553,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -549,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF8B775-73F6-48CF-8D3D-6BC3909EA3F4}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,164 +608,290 @@
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="5">
+        <v>45721</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
       <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="5">
+        <v>45721</v>
+      </c>
+      <c r="H2" s="4">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="5">
+        <v>45721</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
       <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="5">
+        <v>45721</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="5">
+        <v>45721</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
       <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="5">
+        <v>45721</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="5">
+        <v>45721</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
       <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="5">
+        <v>45721</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="5">
+        <v>45721</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="5">
+        <v>45721</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="5">
+        <v>45721</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
       <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="5">
+        <v>45721</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="5">
+        <v>45721</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
       <c r="E8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="5">
+        <v>45721</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="5">
+        <v>45721</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
       <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="5">
+        <v>45721</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="5">
+        <v>45721</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
       <c r="E10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="5">
+        <v>45721</v>
+      </c>
+      <c r="H10" s="4">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="5">
-        <v>45693</v>
+        <v>31</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="C11" s="5">
-        <v>45693</v>
+        <v>45721</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="5">
-        <v>45721</v>
+        <v>10</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="G11" s="5">
         <v>45721</v>
@@ -762,13 +900,13 @@
         <v>1</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="5">
         <v>45693</v>
@@ -798,7 +936,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="5">
         <v>45693</v>
@@ -828,7 +966,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="5">
         <v>45693</v>
@@ -858,7 +996,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="5">
         <v>45693</v>
@@ -888,7 +1026,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="5">
         <v>45693</v>
@@ -918,7 +1056,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="5">
         <v>45693</v>
@@ -948,7 +1086,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="5">
         <v>45693</v>
@@ -978,7 +1116,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="5">
         <v>45693</v>
@@ -1008,35 +1146,66 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="5">
+        <v>45693</v>
+      </c>
+      <c r="C20" s="5">
+        <v>45693</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="5">
+        <v>45721</v>
+      </c>
+      <c r="G20" s="5">
+        <v>45721</v>
+      </c>
+      <c r="H20" s="4">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="5">
-        <v>45693</v>
-      </c>
-      <c r="C20" s="5">
-        <v>45693</v>
-      </c>
-      <c r="D20" s="4">
-        <v>1</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="5">
-        <v>45721</v>
-      </c>
-      <c r="G20" s="5">
-        <v>45721</v>
-      </c>
-      <c r="H20" s="4">
-        <v>1</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J20" s="2"/>
+      <c r="B21" s="5">
+        <v>45693</v>
+      </c>
+      <c r="C21" s="5">
+        <v>45693</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="5">
+        <v>45721</v>
+      </c>
+      <c r="G21" s="5">
+        <v>45721</v>
+      </c>
+      <c r="H21" s="4">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>